<commit_message>
Added test index js file. Added additional 7:10 task, and changed other tasks columns since table where slightely changed
</commit_message>
<xml_diff>
--- a/Completed files/Hymer duomenys.xlsx
+++ b/Completed files/Hymer duomenys.xlsx
@@ -468,14 +468,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>126.2</v>
+        <v>138.2</v>
       </c>
       <c r="D2" t="n">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="E2" t="inlineStr"/>
     </row>
@@ -487,14 +487,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>38.1</v>
+        <v>41.9</v>
       </c>
       <c r="D3" t="n">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="inlineStr"/>
     </row>
@@ -506,14 +506,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>44.2</v>
+        <v>45.4</v>
       </c>
       <c r="D4" t="n">
-        <v>6.7</v>
+        <v>7.2</v>
       </c>
       <c r="E4" t="inlineStr"/>
     </row>
@@ -525,14 +525,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-11-06 12:30Vykdomi</t>
+          <t>2024-11-07 14:30Vykdomi</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>60.4</v>
+        <v>62.8</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -544,14 +544,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>88.40000000000001</v>
+        <v>88.59999999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>7.5</v>
+        <v>8.1</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -563,12 +563,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>6.8</v>
+        <v>7.3</v>
       </c>
       <c r="E7" t="inlineStr"/>
     </row>
@@ -580,14 +580,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>71.90000000000001</v>
+        <v>74.2</v>
       </c>
       <c r="D8" t="n">
-        <v>6.7</v>
+        <v>7.2</v>
       </c>
       <c r="E8" t="inlineStr"/>
     </row>
@@ -599,11 +599,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>109.5</v>
+        <v>109.8</v>
       </c>
       <c r="D9" t="n">
         <v>8.199999999999999</v>
@@ -618,14 +618,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>90.3</v>
+        <v>90.40000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>6.5</v>
+        <v>6.9</v>
       </c>
       <c r="E10" t="inlineStr"/>
     </row>
@@ -637,14 +637,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>139.8</v>
+        <v>137.6</v>
       </c>
       <c r="D11" t="n">
-        <v>9.5</v>
+        <v>9.9</v>
       </c>
       <c r="E11" t="inlineStr"/>
     </row>
@@ -656,12 +656,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>8.300000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="E12" t="inlineStr"/>
     </row>
@@ -673,14 +673,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>94.90000000000001</v>
+        <v>107.8</v>
       </c>
       <c r="D13" t="n">
-        <v>7.7</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E13" t="inlineStr"/>
     </row>
@@ -692,14 +692,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>45.8</v>
+        <v>46.1</v>
       </c>
       <c r="D14" t="n">
-        <v>8.199999999999999</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
@@ -711,14 +711,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>206.9</v>
+        <v>200.3</v>
       </c>
       <c r="D15" t="n">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="E15" t="inlineStr"/>
     </row>
@@ -730,14 +730,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>11.6</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="E16" t="inlineStr"/>
     </row>
@@ -749,14 +749,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>14.6</v>
+        <v>18.9</v>
       </c>
       <c r="D17" t="n">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
       <c r="E17" t="inlineStr"/>
     </row>
@@ -768,14 +768,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>57</v>
+        <v>59.5</v>
       </c>
       <c r="D18" t="n">
-        <v>9.4</v>
+        <v>9</v>
       </c>
       <c r="E18" t="inlineStr"/>
     </row>
@@ -787,12 +787,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>7.8</v>
+        <v>7.4</v>
       </c>
       <c r="E19" t="inlineStr"/>
     </row>
@@ -804,11 +804,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>71</v>
+        <v>70.8</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
@@ -821,14 +821,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>90.90000000000001</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="D21" t="n">
-        <v>7.7</v>
+        <v>7.4</v>
       </c>
       <c r="E21" t="inlineStr"/>
     </row>
@@ -840,11 +840,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>93</v>
+        <v>89.90000000000001</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
@@ -857,11 +857,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>139.7</v>
+        <v>138.9</v>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
@@ -874,11 +874,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>63.8</v>
+        <v>63.6</v>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
@@ -891,14 +891,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>113.8</v>
+        <v>114.1</v>
       </c>
       <c r="D25" t="n">
-        <v>7.6</v>
+        <v>7.5</v>
       </c>
       <c r="E25" t="inlineStr"/>
     </row>
@@ -910,14 +910,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>126.9</v>
+        <v>126.6</v>
       </c>
       <c r="D26" t="n">
-        <v>6.3</v>
+        <v>6.1</v>
       </c>
       <c r="E26" t="inlineStr"/>
     </row>
@@ -929,14 +929,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>96</v>
+        <v>96.3</v>
       </c>
       <c r="D27" t="n">
-        <v>6.2</v>
+        <v>5.6</v>
       </c>
       <c r="E27" t="inlineStr"/>
     </row>
@@ -948,14 +948,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>18.4</v>
+        <v>18.1</v>
       </c>
       <c r="D28" t="n">
-        <v>6.8</v>
+        <v>6</v>
       </c>
       <c r="E28" t="inlineStr"/>
     </row>
@@ -967,14 +967,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>42.1</v>
+        <v>48.5</v>
       </c>
       <c r="D29" t="n">
-        <v>6.5</v>
+        <v>6.1</v>
       </c>
       <c r="E29" t="inlineStr"/>
     </row>
@@ -986,11 +986,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>88.3</v>
+        <v>88.8</v>
       </c>
       <c r="D30" t="n">
         <v>6.6</v>
@@ -1005,14 +1005,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>300.1</v>
+        <v>298.9</v>
       </c>
       <c r="D31" t="n">
-        <v>7.5</v>
+        <v>7.2</v>
       </c>
       <c r="E31" t="inlineStr"/>
     </row>
@@ -1024,14 +1024,14 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>230.1</v>
+        <v>230.5</v>
       </c>
       <c r="D32" t="n">
-        <v>6.4</v>
+        <v>6.8</v>
       </c>
       <c r="E32" t="inlineStr"/>
     </row>
@@ -1043,14 +1043,14 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>248.2</v>
+        <v>244.5</v>
       </c>
       <c r="D33" t="n">
-        <v>10.3</v>
+        <v>10.4</v>
       </c>
       <c r="E33" t="inlineStr"/>
     </row>
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>31.3</v>
+        <v>31.5</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
@@ -1079,14 +1079,14 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C35" t="n">
         <v>79</v>
       </c>
       <c r="D35" t="n">
-        <v>6.7</v>
+        <v>7.1</v>
       </c>
       <c r="E35" t="inlineStr"/>
     </row>
@@ -1098,14 +1098,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>190.4</v>
+        <v>185.5</v>
       </c>
       <c r="D36" t="n">
-        <v>6.1</v>
+        <v>6.4</v>
       </c>
       <c r="E36" t="inlineStr"/>
     </row>
@@ -1117,14 +1117,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="D37" t="n">
-        <v>6.6</v>
+        <v>7.1</v>
       </c>
       <c r="E37" t="inlineStr"/>
     </row>
@@ -1136,14 +1136,14 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>22.9</v>
+        <v>23.2</v>
       </c>
       <c r="D38" t="n">
-        <v>7</v>
+        <v>7.1</v>
       </c>
       <c r="E38" t="inlineStr"/>
     </row>
@@ -1155,14 +1155,14 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>54.2</v>
+        <v>52.5</v>
       </c>
       <c r="D39" t="n">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
       <c r="E39" t="inlineStr"/>
     </row>
@@ -1174,14 +1174,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>61.8</v>
+        <v>60.4</v>
       </c>
       <c r="D40" t="n">
-        <v>8.699999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="E40" t="inlineStr"/>
     </row>
@@ -1193,11 +1193,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>17.7</v>
+        <v>17.5</v>
       </c>
       <c r="D41" t="n">
         <v>9.199999999999999</v>
@@ -1212,12 +1212,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
-        <v>6.4</v>
+        <v>7.2</v>
       </c>
       <c r="E42" t="inlineStr"/>
     </row>
@@ -1229,14 +1229,14 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>115</v>
+        <v>121.4</v>
       </c>
       <c r="D43" t="n">
-        <v>5.6</v>
+        <v>7</v>
       </c>
       <c r="E43" t="inlineStr"/>
     </row>
@@ -1248,12 +1248,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
-        <v>7</v>
+        <v>7.3</v>
       </c>
       <c r="E44" t="inlineStr"/>
     </row>
@@ -1265,14 +1265,14 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>100.4</v>
+        <v>100.1</v>
       </c>
       <c r="D45" t="n">
-        <v>6.2</v>
+        <v>6.9</v>
       </c>
       <c r="E45" t="inlineStr"/>
     </row>
@@ -1284,14 +1284,14 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3</v>
+        <v>2.3</v>
       </c>
       <c r="D46" t="n">
-        <v>9.5</v>
+        <v>9.9</v>
       </c>
       <c r="E46" t="inlineStr"/>
     </row>
@@ -1303,14 +1303,14 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>22.3</v>
+        <v>19.7</v>
       </c>
       <c r="D47" t="n">
-        <v>8</v>
+        <v>8.1</v>
       </c>
       <c r="E47" t="inlineStr"/>
     </row>
@@ -1322,14 +1322,14 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>18.4</v>
+        <v>13.9</v>
       </c>
       <c r="D48" t="n">
-        <v>7.2</v>
+        <v>6.5</v>
       </c>
       <c r="E48" t="inlineStr"/>
     </row>
@@ -1341,14 +1341,14 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>116.1</v>
+        <v>110.4</v>
       </c>
       <c r="D49" t="n">
-        <v>6.8</v>
+        <v>7.9</v>
       </c>
       <c r="E49" t="inlineStr"/>
     </row>
@@ -1360,14 +1360,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>22.5</v>
+        <v>20.2</v>
       </c>
       <c r="D50" t="n">
-        <v>6.6</v>
+        <v>6.9</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
@@ -1379,14 +1379,14 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>7.5</v>
+        <v>14.2</v>
       </c>
       <c r="D51" t="n">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -1398,14 +1398,14 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>96.90000000000001</v>
+        <v>95.90000000000001</v>
       </c>
       <c r="D52" t="n">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="E52" t="inlineStr"/>
     </row>
@@ -1417,14 +1417,14 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>534.5</v>
+        <v>525.8</v>
       </c>
       <c r="D53" t="n">
-        <v>6.9</v>
+        <v>7.3</v>
       </c>
       <c r="E53" t="inlineStr"/>
     </row>
@@ -1436,14 +1436,14 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>70.5</v>
+        <v>68.5</v>
       </c>
       <c r="D54" t="n">
-        <v>7.7</v>
+        <v>8</v>
       </c>
       <c r="E54" t="inlineStr"/>
     </row>
@@ -1455,14 +1455,14 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>152.5</v>
+        <v>143.9</v>
       </c>
       <c r="D55" t="n">
-        <v>7</v>
+        <v>7.3</v>
       </c>
       <c r="E55" t="inlineStr"/>
     </row>
@@ -1474,14 +1474,14 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>496.7</v>
+        <v>507.3</v>
       </c>
       <c r="D56" t="n">
-        <v>6.8</v>
+        <v>6.5</v>
       </c>
       <c r="E56" t="inlineStr"/>
     </row>
@@ -1493,14 +1493,14 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>490.9</v>
+        <v>503.2</v>
       </c>
       <c r="D57" t="n">
-        <v>5.9</v>
+        <v>5.4</v>
       </c>
       <c r="E57" t="inlineStr"/>
     </row>
@@ -1512,14 +1512,14 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>111.4</v>
+        <v>104</v>
       </c>
       <c r="D58" t="n">
-        <v>7.7</v>
+        <v>7.9</v>
       </c>
       <c r="E58" t="inlineStr"/>
     </row>
@@ -1531,14 +1531,14 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>147.5</v>
+        <v>141.2</v>
       </c>
       <c r="D59" t="n">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="E59" t="inlineStr"/>
     </row>
@@ -1550,14 +1550,14 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>99.40000000000001</v>
+        <v>101.9</v>
       </c>
       <c r="D60" t="n">
-        <v>7.8</v>
+        <v>8</v>
       </c>
       <c r="E60" t="inlineStr"/>
     </row>
@@ -1569,14 +1569,14 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>138.4</v>
+        <v>137</v>
       </c>
       <c r="D61" t="n">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="E61" t="inlineStr"/>
     </row>
@@ -1588,14 +1588,14 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>23.1</v>
+        <v>27.3</v>
       </c>
       <c r="D62" t="n">
-        <v>7.9</v>
+        <v>8</v>
       </c>
       <c r="E62" t="inlineStr"/>
     </row>
@@ -1607,14 +1607,14 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2024-11-06 13:30Vykdomi</t>
+          <t>2024-11-07 15:30Vykdomi</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>82.5</v>
+        <v>83.59999999999999</v>
       </c>
       <c r="D63" t="n">
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="E63" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Changed original js with tasks column  changes
</commit_message>
<xml_diff>
--- a/Completed files/Hymer duomenys.xlsx
+++ b/Completed files/Hymer duomenys.xlsx
@@ -468,14 +468,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>138.2</v>
+        <v>136.6</v>
       </c>
       <c r="D2" t="n">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="E2" t="inlineStr"/>
     </row>
@@ -487,14 +487,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>41.9</v>
+        <v>53.2</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="E3" t="inlineStr"/>
     </row>
@@ -506,14 +506,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>45.4</v>
+        <v>44.8</v>
       </c>
       <c r="D4" t="n">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="E4" t="inlineStr"/>
     </row>
@@ -525,14 +525,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-11-07 14:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>62.8</v>
+        <v>63</v>
       </c>
       <c r="D5" t="n">
-        <v>7.5</v>
+        <v>7.8</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
@@ -544,14 +544,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>88.59999999999999</v>
+        <v>88.7</v>
       </c>
       <c r="D6" t="n">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
@@ -563,12 +563,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>7.3</v>
+        <v>7.1</v>
       </c>
       <c r="E7" t="inlineStr"/>
     </row>
@@ -580,14 +580,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>74.2</v>
+        <v>73.2</v>
       </c>
       <c r="D8" t="n">
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="E8" t="inlineStr"/>
     </row>
@@ -599,14 +599,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>109.8</v>
+        <v>109</v>
       </c>
       <c r="D9" t="n">
-        <v>8.199999999999999</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E9" t="inlineStr"/>
     </row>
@@ -618,14 +618,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>90.40000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="D10" t="n">
-        <v>6.9</v>
+        <v>7.1</v>
       </c>
       <c r="E10" t="inlineStr"/>
     </row>
@@ -637,14 +637,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>137.6</v>
+        <v>136.7</v>
       </c>
       <c r="D11" t="n">
-        <v>9.9</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E11" t="inlineStr"/>
     </row>
@@ -656,12 +656,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>8.4</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E12" t="inlineStr"/>
     </row>
@@ -673,14 +673,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>107.8</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="D13" t="n">
-        <v>8.199999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="E13" t="inlineStr"/>
     </row>
@@ -692,14 +692,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>46.1</v>
+        <v>33.1</v>
       </c>
       <c r="D14" t="n">
-        <v>8.699999999999999</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E14" t="inlineStr"/>
     </row>
@@ -711,11 +711,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>200.3</v>
+        <v>197.9</v>
       </c>
       <c r="D15" t="n">
         <v>7.3</v>
@@ -730,11 +730,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>12.7</v>
       </c>
       <c r="D16" t="n">
         <v>6.5</v>
@@ -749,14 +749,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>18.9</v>
+        <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
       <c r="E17" t="inlineStr"/>
     </row>
@@ -768,14 +768,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>59.5</v>
+        <v>64.2</v>
       </c>
       <c r="D18" t="n">
-        <v>9</v>
+        <v>8.9</v>
       </c>
       <c r="E18" t="inlineStr"/>
     </row>
@@ -787,12 +787,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>7.4</v>
+        <v>7.7</v>
       </c>
       <c r="E19" t="inlineStr"/>
     </row>
@@ -804,11 +804,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>70.8</v>
+        <v>71.2</v>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
@@ -821,14 +821,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>91.59999999999999</v>
+        <v>92.5</v>
       </c>
       <c r="D21" t="n">
-        <v>7.4</v>
+        <v>7.6</v>
       </c>
       <c r="E21" t="inlineStr"/>
     </row>
@@ -840,11 +840,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>89.90000000000001</v>
+        <v>88.8</v>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
@@ -857,7 +857,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -874,7 +874,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -891,14 +891,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>114.1</v>
+        <v>114.8</v>
       </c>
       <c r="D25" t="n">
-        <v>7.5</v>
+        <v>7.6</v>
       </c>
       <c r="E25" t="inlineStr"/>
     </row>
@@ -910,14 +910,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>126.6</v>
+        <v>125.6</v>
       </c>
       <c r="D26" t="n">
-        <v>6.1</v>
+        <v>6.3</v>
       </c>
       <c r="E26" t="inlineStr"/>
     </row>
@@ -929,14 +929,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>96.3</v>
+        <v>98.09999999999999</v>
       </c>
       <c r="D27" t="n">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="E27" t="inlineStr"/>
     </row>
@@ -948,14 +948,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>18.1</v>
+        <v>18</v>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>6.3</v>
       </c>
       <c r="E28" t="inlineStr"/>
     </row>
@@ -967,14 +967,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>48.5</v>
+        <v>42.1</v>
       </c>
       <c r="D29" t="n">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="E29" t="inlineStr"/>
     </row>
@@ -986,14 +986,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>88.8</v>
+        <v>87.8</v>
       </c>
       <c r="D30" t="n">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
       <c r="E30" t="inlineStr"/>
     </row>
@@ -1005,11 +1005,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>298.9</v>
+        <v>300.4</v>
       </c>
       <c r="D31" t="n">
         <v>7.2</v>
@@ -1024,11 +1024,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>230.5</v>
+        <v>227.6</v>
       </c>
       <c r="D32" t="n">
         <v>6.8</v>
@@ -1043,14 +1043,14 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>244.5</v>
+        <v>246.8</v>
       </c>
       <c r="D33" t="n">
-        <v>10.4</v>
+        <v>10.5</v>
       </c>
       <c r="E33" t="inlineStr"/>
     </row>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1079,11 +1079,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>79</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="D35" t="n">
         <v>7.1</v>
@@ -1098,14 +1098,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>185.5</v>
+        <v>185.3</v>
       </c>
       <c r="D36" t="n">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
       <c r="E36" t="inlineStr"/>
     </row>
@@ -1117,14 +1117,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2.8</v>
+        <v>2.3</v>
       </c>
       <c r="D37" t="n">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="E37" t="inlineStr"/>
     </row>
@@ -1136,14 +1136,14 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>23.2</v>
+        <v>20.5</v>
       </c>
       <c r="D38" t="n">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="E38" t="inlineStr"/>
     </row>
@@ -1155,14 +1155,14 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>52.5</v>
+        <v>58</v>
       </c>
       <c r="D39" t="n">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
       <c r="E39" t="inlineStr"/>
     </row>
@@ -1174,14 +1174,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>60.4</v>
+        <v>59.7</v>
       </c>
       <c r="D40" t="n">
-        <v>9.1</v>
+        <v>9</v>
       </c>
       <c r="E40" t="inlineStr"/>
     </row>
@@ -1193,14 +1193,14 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>17.5</v>
+        <v>16.9</v>
       </c>
       <c r="D41" t="n">
-        <v>9.199999999999999</v>
+        <v>9</v>
       </c>
       <c r="E41" t="inlineStr"/>
     </row>
@@ -1212,12 +1212,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="E42" t="inlineStr"/>
     </row>
@@ -1229,14 +1229,14 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>121.4</v>
+        <v>118.4</v>
       </c>
       <c r="D43" t="n">
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="E43" t="inlineStr"/>
     </row>
@@ -1248,12 +1248,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
-        <v>7.3</v>
+        <v>7.5</v>
       </c>
       <c r="E44" t="inlineStr"/>
     </row>
@@ -1265,14 +1265,14 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>100.1</v>
+        <v>99.3</v>
       </c>
       <c r="D45" t="n">
-        <v>6.9</v>
+        <v>7</v>
       </c>
       <c r="E45" t="inlineStr"/>
     </row>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1303,14 +1303,14 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>19.7</v>
+        <v>19.6</v>
       </c>
       <c r="D47" t="n">
-        <v>8.1</v>
+        <v>7.9</v>
       </c>
       <c r="E47" t="inlineStr"/>
     </row>
@@ -1322,14 +1322,14 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>13.9</v>
+        <v>19.5</v>
       </c>
       <c r="D48" t="n">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="E48" t="inlineStr"/>
     </row>
@@ -1341,14 +1341,14 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>110.4</v>
+        <v>123.4</v>
       </c>
       <c r="D49" t="n">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="E49" t="inlineStr"/>
     </row>
@@ -1360,14 +1360,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>20.2</v>
+        <v>19</v>
       </c>
       <c r="D50" t="n">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="E50" t="inlineStr"/>
     </row>
@@ -1379,14 +1379,14 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>14.2</v>
+        <v>17.3</v>
       </c>
       <c r="D51" t="n">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="E51" t="inlineStr"/>
     </row>
@@ -1398,11 +1398,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>95.90000000000001</v>
+        <v>95.2</v>
       </c>
       <c r="D52" t="n">
         <v>7.5</v>
@@ -1417,11 +1417,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>525.8</v>
+        <v>523.3</v>
       </c>
       <c r="D53" t="n">
         <v>7.3</v>
@@ -1436,14 +1436,14 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>68.5</v>
+        <v>68.2</v>
       </c>
       <c r="D54" t="n">
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="E54" t="inlineStr"/>
     </row>
@@ -1455,11 +1455,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>143.9</v>
+        <v>141.4</v>
       </c>
       <c r="D55" t="n">
         <v>7.3</v>
@@ -1474,14 +1474,14 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>507.3</v>
+        <v>517.8</v>
       </c>
       <c r="D56" t="n">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="E56" t="inlineStr"/>
     </row>
@@ -1493,14 +1493,14 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>503.2</v>
+        <v>511.7</v>
       </c>
       <c r="D57" t="n">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
       <c r="E57" t="inlineStr"/>
     </row>
@@ -1512,14 +1512,14 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>104</v>
+        <v>101.8</v>
       </c>
       <c r="D58" t="n">
-        <v>7.9</v>
+        <v>8</v>
       </c>
       <c r="E58" t="inlineStr"/>
     </row>
@@ -1531,11 +1531,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>141.2</v>
+        <v>140.8</v>
       </c>
       <c r="D59" t="n">
         <v>9</v>
@@ -1550,11 +1550,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>101.9</v>
+        <v>95.8</v>
       </c>
       <c r="D60" t="n">
         <v>8</v>
@@ -1569,14 +1569,14 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>137</v>
+        <v>136.7</v>
       </c>
       <c r="D61" t="n">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="E61" t="inlineStr"/>
     </row>
@@ -1588,14 +1588,14 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>27.3</v>
+        <v>23.2</v>
       </c>
       <c r="D62" t="n">
-        <v>8</v>
+        <v>7.9</v>
       </c>
       <c r="E62" t="inlineStr"/>
     </row>
@@ -1607,14 +1607,14 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2024-11-07 15:30Vykdomi</t>
+          <t>2024-11-08 04:30Vykdomi</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>83.59999999999999</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="D63" t="n">
-        <v>8.4</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E63" t="inlineStr"/>
     </row>

</xml_diff>